<commit_message>
bug fixed in Database Table ID
</commit_message>
<xml_diff>
--- a/experiment_results/TLDR Experiment/experiment 1/TLDR_EXP_1_APACHE_COMMON_IO.xlsx
+++ b/experiment_results/TLDR Experiment/experiment 1/TLDR_EXP_1_APACHE_COMMON_IO.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demigorgan/TLDR_EXP/Ekstazi_log/experiment 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demigorgan/Documents/workspace/tldr/experiment_results/TLDR Experiment/experiment 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-35280" yWindow="-1080" windowWidth="31160" windowHeight="17020" tabRatio="500"/>
+    <workbookView xWindow="-73560" yWindow="100" windowWidth="31160" windowHeight="17020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -138,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,6 +159,22 @@
       <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -182,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,6 +213,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +501,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,7 +682,7 @@
         <v>256</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F4:F23" si="2">100*(E5/C5)</f>
+        <f t="shared" ref="F5:F22" si="2">100*(E5/C5)</f>
         <v>34.178905206942588</v>
       </c>
       <c r="G5" s="1">
@@ -1298,166 +1322,166 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="A21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="7">
         <v>1018</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="7">
         <v>121</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="7">
         <v>237</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="7">
         <f t="shared" si="2"/>
         <v>23.280943025540275</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="7">
         <v>1.07</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="7">
         <v>13.371</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="7">
         <f t="shared" si="0"/>
         <v>14.441000000000001</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="7">
         <v>744</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="7">
         <f t="shared" si="1"/>
         <v>73.084479371316306</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L21" s="7">
         <v>114.75</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="A22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="7">
         <v>1018</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="7">
         <v>109</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="7">
         <v>209</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="7">
         <f t="shared" si="2"/>
         <v>20.530451866404714</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="7">
         <v>1.1339999999999999</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="7">
         <v>13.266</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="7">
         <f t="shared" si="0"/>
         <v>14.4</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="7">
         <v>717</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="7">
         <f t="shared" si="1"/>
         <v>70.43222003929273</v>
       </c>
-      <c r="L22" s="1">
+      <c r="L22" s="7">
         <v>58.889000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="23" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="9">
         <v>1027</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="9">
         <v>125</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="9">
         <v>499</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="9">
         <f>100*(E23/C23)</f>
         <v>48.588120740019477</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="9">
         <v>2.1987999999999999</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="9">
         <v>32.216999999999999</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="9">
         <f t="shared" si="0"/>
         <v>34.415799999999997</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="9">
         <v>928</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="9">
         <f t="shared" si="1"/>
         <v>90.360272638753642</v>
       </c>
-      <c r="L23" s="1">
+      <c r="L23" s="9">
         <v>128.87700000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="24" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="9">
         <v>1032</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="9">
         <v>101</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="9">
         <v>28</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="9">
         <f>100*(E24/C24)</f>
         <v>2.7131782945736433</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="9">
         <v>0.73399999999999999</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="9">
         <v>9.9749999999999996</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="9">
         <f t="shared" si="0"/>
         <v>10.709</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="9">
         <v>555</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="9">
         <f t="shared" si="1"/>
         <v>53.779069767441854</v>
       </c>
-      <c r="L24" s="1">
+      <c r="L24" s="9">
         <v>95.974999999999994</v>
       </c>
     </row>

</xml_diff>